<commit_message>
Done the changes as suggested on last Demo. Third Commit.
</commit_message>
<xml_diff>
--- a/GroceryAppProject/src/main/resources/Excelfiles/DataProvider.xlsx
+++ b/GroceryAppProject/src/main/resources/Excelfiles/DataProvider.xlsx
@@ -3,18 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Testing\Testing Course\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15555" windowHeight="3075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ExpectedResultSheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Usernam</t>
   </si>
@@ -39,16 +36,172 @@
   </si>
   <si>
     <t>veena</t>
+  </si>
+  <si>
+    <t>Constatnt Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>EXPECTEDOFFERCOODEALERTMESSAGE</t>
+  </si>
+  <si>
+    <t>Alert Offer Created Successfully</t>
+  </si>
+  <si>
+    <r>
+      <t>EXPECTEDALERTMESSAGEOFDELIVERYBOYDETAILS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>Alert Delivery Boy Details Created Successfully</t>
+  </si>
+  <si>
+    <t>EXPECTEDTOOLTIPVALUES</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>EXPECTEDVALUEFROMDROPDOWNGROUP</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>EXPECTEDINVALIDLOGINALERT</t>
+  </si>
+  <si>
+    <t>Alert Invalid Username/Password</t>
+  </si>
+  <si>
+    <t>EXPECTEDBGCOLORSIGNINBTN</t>
+  </si>
+  <si>
+    <t>rgba(52, 58, 64, 1)</t>
+  </si>
+  <si>
+    <t>EXPECTEDTEXTOFSIGNINBUTTON</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t>EXPECTEDURLOFSIGNINPAGE</t>
+  </si>
+  <si>
+    <t>https://groceryapp.uniqassosiates.com/admin/login</t>
+  </si>
+  <si>
+    <t>EXPECTEDRESULTOFCREATEDSLIDER</t>
+  </si>
+  <si>
+    <t>Alert Slider Created Successfully</t>
+  </si>
+  <si>
+    <t>EXPECTEDTITLEOFMANAGESLIDER</t>
+  </si>
+  <si>
+    <t>Add Slider | 7rmart supermarket</t>
+  </si>
+  <si>
+    <t>EXPECTEDRGBCOLORFORMANAGESLIDER</t>
+  </si>
+  <si>
+    <t>rgba(0, 0, 0, 0)</t>
+  </si>
+  <si>
+    <t>EXPECTEDVALUEINDROPDOWNSTATUS</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>EXPECTEDUSERNAMEFORMANAGEUSERPAGE</t>
+  </si>
+  <si>
+    <t>Ruby Varghese</t>
+  </si>
+  <si>
+    <t>EXPECTEDURLOFADMINPAGE</t>
+  </si>
+  <si>
+    <t>EXPECTEDALERTINADMINUSERSPAGE</t>
+  </si>
+  <si>
+    <t>Alert User Created Successfully</t>
+  </si>
+  <si>
+    <t>EXPECTEDSELECTEDVALUEFROMTHEDROPDOWNPAYMNETMODE</t>
+  </si>
+  <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>EXPECTEDBACKGROUNDCOLOUROFSEARCHBUTTONINLISTLOCATION</t>
+  </si>
+  <si>
+    <t>rgba(0, 123, 255, 1)</t>
+  </si>
+  <si>
+    <t>EXPECTEDRESULTSELECTEDSTATEINADDLOCATIONPAGE</t>
+  </si>
+  <si>
+    <t>Aberdeen</t>
+  </si>
+  <si>
+    <t>ALERTMESSAGEOFADDLOCATION</t>
+  </si>
+  <si>
+    <t>Alert Location Created Successfully</t>
+  </si>
+  <si>
+    <t>COMMONALERTMESSAGE</t>
+  </si>
+  <si>
+    <t>Expected result not matched</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF0000C0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,13 +224,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -395,4 +565,196 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B15" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>